<commit_message>
There is another bug :(
</commit_message>
<xml_diff>
--- a/Logs 2021-02-19.xlsx
+++ b/Logs 2021-02-19.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="10">
   <si>
     <t>Cache</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>ÿþG_x0000_C_x0000_5_x0000_1_x0000_C_x0000_1_x0000_5_x0000_</t>
+    <t>some</t>
   </si>
   <si>
     <t>_x0000_2_x0000_0_x0000_2_x0000_1_x0000_-_x0000_0_x0000_2_x0000_-_x0000_1_x0000_9_x0000_</t>
@@ -40,34 +40,31 @@
     <t>_x0000_1_x0000_9_x0000_:_x0000_1_x0000_3_x0000__x0000_</t>
   </si>
   <si>
-    <t>_x0000_F_x0000_o_x0000_u_x0000_n_x0000_d_x0000_ _x0000_i_x0000_t_x0000_</t>
+    <t>_x0000_F_x0000_o_x0000_u_x0000_n_x0000_d_x0000__x0000_i_x0000_t_x0000_</t>
   </si>
   <si>
     <t xml:space="preserve">_x0000_"_x0000_"_x0000_
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_x0000_
-</t>
-  </si>
-  <si>
-    <t>_x0000_G_x0000_C_x0000_5_x0000_1_x0000_C_x0000_1_x0000_5_x0000_</t>
-  </si>
-  <si>
-    <t>_x0000_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,13 +84,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -386,37 +389,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>10</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>11</v>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -432,13 +447,25 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>10</v>
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>11</v>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -454,13 +481,25 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>10</v>
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>11</v>
+      <c r="A7" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -476,13 +515,25 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>10</v>
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>11</v>
+      <c r="A9" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -498,13 +549,25 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>10</v>
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>11</v>
+      <c r="A11" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -520,13 +583,25 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>10</v>
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>11</v>
+      <c r="A13" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -542,13 +617,25 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>10</v>
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>11</v>
+      <c r="A15" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -564,158 +651,29 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>12</v>
+      <c r="A16" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A7" r:id="rId7"/>
+    <hyperlink ref="A8" r:id="rId8"/>
+    <hyperlink ref="A9" r:id="rId9"/>
+    <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A11" r:id="rId11"/>
+    <hyperlink ref="A12" r:id="rId12"/>
+    <hyperlink ref="A13" r:id="rId13"/>
+    <hyperlink ref="A14" r:id="rId14"/>
+    <hyperlink ref="A15" r:id="rId15"/>
+    <hyperlink ref="A16" r:id="rId16"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>